<commit_message>
start work on get-hplldpneighbor
</commit_message>
<xml_diff>
--- a/ObjectHierarchy.xlsx
+++ b/ObjectHierarchy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>int</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>array[string]</t>
-  </si>
-  <si>
     <t>DhcpRelayEnabled</t>
   </si>
   <si>
@@ -50,6 +47,42 @@
   </si>
   <si>
     <t>DhcpRelayList</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>PimSmEnabled</t>
+  </si>
+  <si>
+    <t>LinkAggMode</t>
+  </si>
+  <si>
+    <t>MadEnabled</t>
+  </si>
+  <si>
+    <t>PermittedVlans</t>
+  </si>
+  <si>
+    <t>list&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>list&lt;int&gt;</t>
+  </si>
+  <si>
+    <t>Pvid</t>
+  </si>
+  <si>
+    <t>IsShutdown</t>
+  </si>
+  <si>
+    <t>PortLinkType</t>
+  </si>
+  <si>
+    <t>PortLinkMode</t>
+  </si>
+  <si>
+    <t>LinkAggGroup</t>
   </si>
 </sst>
 </file>
@@ -391,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A2:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,18 +477,132 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>